<commit_message>
Added a simply script to re-number the json index (value in the key-value pair) Note that this does not change any result in current data collection, this is just to make the dataset more formated
- Added spreadsheet for hammer (not yet label)
</commit_message>
<xml_diff>
--- a/spreadsheet/web_scrape_bakingtray.xlsx
+++ b/spreadsheet/web_scrape_bakingtray.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamlam/Desktop/FYP/ObjectPropertiesInformationExtraction/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6BA805-72A8-244C-AD3A-1281BF6F6CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2886580E-188D-DB44-B0E1-64420BBB3497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="33500" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="33500" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="438">
   <si>
     <t xml:space="preserve">Prochef KB1004 Large Baking/Oven Tray, Premium Quality, Easy to Clean, Teflon Innovations Non-Stick Silicone Coating,Grey
 Colour Grey
@@ -2556,9 +2556,6 @@
     <t>12.59</t>
   </si>
   <si>
-    <t>318</t>
-  </si>
-  <si>
     <t>28</t>
   </si>
   <si>
@@ -2601,18 +2598,12 @@
     <t>28.9</t>
   </si>
   <si>
-    <t>465</t>
-  </si>
-  <si>
     <t>42</t>
   </si>
   <si>
     <t>38.1</t>
   </si>
   <si>
-    <t>45.5</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -2727,9 +2718,6 @@
     <t>21.2</t>
   </si>
   <si>
-    <t>455</t>
-  </si>
-  <si>
     <t>34.2</t>
   </si>
   <si>
@@ -2766,9 +2754,6 @@
     <t>11.81</t>
   </si>
   <si>
-    <t>216</t>
-  </si>
-  <si>
     <t>27.18</t>
   </si>
   <si>
@@ -2799,9 +2784,6 @@
     <t>12.7</t>
   </si>
   <si>
-    <t>375</t>
-  </si>
-  <si>
     <t>26.9</t>
   </si>
   <si>
@@ -2889,9 +2871,6 @@
     <t>23.5</t>
   </si>
   <si>
-    <t>377</t>
-  </si>
-  <si>
     <t>24.6</t>
   </si>
   <si>
@@ -2934,9 +2913,6 @@
     <t>2.16</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>3.3</t>
   </si>
   <si>
@@ -3043,9 +3019,6 @@
   </si>
   <si>
     <t>1.2</t>
-  </si>
-  <si>
-    <t>60</t>
   </si>
   <si>
     <t>6.1</t>
@@ -3466,8 +3439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="H141" sqref="H141"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3484,28 +3457,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -3528,10 +3501,10 @@
         <v>254</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
@@ -3554,10 +3527,10 @@
         <v>255</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -3580,10 +3553,10 @@
         <v>256</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -3609,7 +3582,7 @@
         <v>259</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="395" x14ac:dyDescent="0.2">
@@ -3632,10 +3605,10 @@
         <v>258</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -3661,7 +3634,7 @@
         <v>257</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -3684,10 +3657,10 @@
         <v>260</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="272" x14ac:dyDescent="0.2">
@@ -3710,10 +3683,10 @@
         <v>261</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="272" x14ac:dyDescent="0.2">
@@ -3736,10 +3709,10 @@
         <v>262</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -3762,10 +3735,10 @@
         <v>263</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -3788,10 +3761,10 @@
         <v>258</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -3814,10 +3787,10 @@
         <v>264</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -3840,10 +3813,10 @@
         <v>265</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -3869,7 +3842,7 @@
         <v>266</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -3892,10 +3865,10 @@
         <v>266</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
@@ -3918,10 +3891,10 @@
         <v>267</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -3947,7 +3920,7 @@
         <v>259</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="240" x14ac:dyDescent="0.2">
@@ -3970,10 +3943,10 @@
         <v>268</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -3996,10 +3969,10 @@
         <v>269</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -4022,10 +3995,10 @@
         <v>270</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="144" x14ac:dyDescent="0.2">
@@ -4044,14 +4017,14 @@
       <c r="E22" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>397</v>
+      <c r="F22" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="G22" s="2">
+        <v>22</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.9</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -4071,13 +4044,13 @@
         <v>135</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="128" x14ac:dyDescent="0.2">
@@ -4097,13 +4070,13 @@
         <v>135</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -4123,13 +4096,13 @@
         <v>135</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -4149,13 +4122,13 @@
         <v>251</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -4175,13 +4148,13 @@
         <v>135</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -4204,10 +4177,10 @@
         <v>266</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -4227,13 +4200,13 @@
         <v>135</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -4253,13 +4226,13 @@
         <v>135</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -4279,13 +4252,13 @@
         <v>135</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -4305,13 +4278,13 @@
         <v>135</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -4331,13 +4304,13 @@
         <v>251</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -4357,13 +4330,13 @@
         <v>135</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -4389,7 +4362,7 @@
         <v>259</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -4409,13 +4382,13 @@
         <v>135</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -4435,13 +4408,13 @@
         <v>252</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -4464,10 +4437,10 @@
         <v>265</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -4487,13 +4460,13 @@
         <v>135</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -4513,13 +4486,13 @@
         <v>135</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -4538,14 +4511,14 @@
       <c r="E41" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>259</v>
+      <c r="F41" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="G41" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="H41" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -4565,13 +4538,13 @@
         <v>135</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="365" x14ac:dyDescent="0.2">
@@ -4591,13 +4564,13 @@
         <v>135</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -4616,14 +4589,14 @@
       <c r="E44" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>274</v>
+      <c r="F44" s="2">
+        <v>43</v>
+      </c>
+      <c r="G44" s="2">
+        <v>47</v>
+      </c>
+      <c r="H44" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -4646,10 +4619,10 @@
         <v>259</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -4669,13 +4642,13 @@
         <v>135</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="240" x14ac:dyDescent="0.2">
@@ -4695,13 +4668,13 @@
         <v>135</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -4727,7 +4700,7 @@
         <v>256</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -4747,13 +4720,13 @@
         <v>135</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>266</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -4773,13 +4746,13 @@
         <v>135</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -4802,10 +4775,10 @@
         <v>265</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -4825,13 +4798,13 @@
         <v>135</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>257</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -4851,13 +4824,13 @@
         <v>135</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -4877,13 +4850,13 @@
         <v>135</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -4903,13 +4876,13 @@
         <v>135</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -4929,13 +4902,13 @@
         <v>135</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>257</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="240" x14ac:dyDescent="0.2">
@@ -4955,13 +4928,13 @@
         <v>135</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -4987,7 +4960,7 @@
         <v>256</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -5007,13 +4980,13 @@
         <v>135</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -5036,10 +5009,10 @@
         <v>256</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -5059,13 +5032,13 @@
         <v>135</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>266</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -5085,13 +5058,13 @@
         <v>135</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -5111,13 +5084,13 @@
         <v>135</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -5137,13 +5110,13 @@
         <v>135</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -5166,10 +5139,10 @@
         <v>265</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -5189,13 +5162,13 @@
         <v>135</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -5215,13 +5188,13 @@
         <v>135</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>257</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -5241,13 +5214,13 @@
         <v>135</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -5267,13 +5240,13 @@
         <v>135</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -5293,13 +5266,13 @@
         <v>135</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>257</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -5322,10 +5295,10 @@
         <v>256</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -5345,13 +5318,13 @@
         <v>135</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
@@ -5371,13 +5344,13 @@
         <v>135</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -5397,13 +5370,13 @@
         <v>135</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="240" x14ac:dyDescent="0.2">
@@ -5423,13 +5396,13 @@
         <v>135</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -5475,13 +5448,13 @@
         <v>135</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>257</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -5501,13 +5474,13 @@
         <v>135</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -5527,13 +5500,13 @@
         <v>135</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -5553,13 +5526,13 @@
         <v>135</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="128" x14ac:dyDescent="0.2">
@@ -5582,10 +5555,10 @@
         <v>264</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -5608,10 +5581,10 @@
         <v>266</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -5631,13 +5604,13 @@
         <v>135</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -5663,7 +5636,7 @@
         <v>259</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -5686,10 +5659,10 @@
         <v>266</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -5709,13 +5682,13 @@
         <v>135</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -5738,10 +5711,10 @@
         <v>266</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -5761,13 +5734,13 @@
         <v>135</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -5790,10 +5763,10 @@
         <v>264</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -5816,10 +5789,10 @@
         <v>256</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -5842,10 +5815,10 @@
         <v>254</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="380" x14ac:dyDescent="0.2">
@@ -5865,13 +5838,13 @@
         <v>135</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -5891,13 +5864,13 @@
         <v>135</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -5917,13 +5890,13 @@
         <v>135</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="350" x14ac:dyDescent="0.2">
@@ -5943,13 +5916,13 @@
         <v>135</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -5969,13 +5942,13 @@
         <v>135</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -5995,13 +5968,13 @@
         <v>135</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -6021,13 +5994,13 @@
         <v>135</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>256</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6047,13 +6020,13 @@
         <v>135</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -6073,13 +6046,13 @@
         <v>135</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -6099,13 +6072,13 @@
         <v>135</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -6125,10 +6098,10 @@
         <v>135</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="H102" s="2" t="s">
         <v>269</v>
@@ -6151,13 +6124,13 @@
         <v>135</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -6177,13 +6150,13 @@
         <v>135</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6203,13 +6176,13 @@
         <v>135</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -6229,13 +6202,13 @@
         <v>135</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="160" x14ac:dyDescent="0.2">
@@ -6281,13 +6254,13 @@
         <v>135</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -6307,13 +6280,13 @@
         <v>135</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -6333,13 +6306,13 @@
         <v>135</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6359,13 +6332,13 @@
         <v>135</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6385,13 +6358,13 @@
         <v>135</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -6411,13 +6384,13 @@
         <v>135</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="240" x14ac:dyDescent="0.2">
@@ -6437,13 +6410,13 @@
         <v>135</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6463,13 +6436,13 @@
         <v>135</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -6489,13 +6462,13 @@
         <v>135</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6518,10 +6491,10 @@
         <v>266</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
@@ -6541,13 +6514,13 @@
         <v>135</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -6567,13 +6540,13 @@
         <v>135</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>265</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="272" x14ac:dyDescent="0.2">
@@ -6596,10 +6569,10 @@
         <v>259</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="256" x14ac:dyDescent="0.2">
@@ -6619,13 +6592,13 @@
         <v>135</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -6648,10 +6621,10 @@
         <v>266</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -6671,13 +6644,13 @@
         <v>253</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="288" x14ac:dyDescent="0.2">
@@ -6697,13 +6670,13 @@
         <v>135</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="320" x14ac:dyDescent="0.2">
@@ -6723,13 +6696,13 @@
         <v>135</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>266</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -6749,13 +6722,13 @@
         <v>135</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -6775,13 +6748,13 @@
         <v>135</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="176" x14ac:dyDescent="0.2">
@@ -6801,13 +6774,13 @@
         <v>135</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="208" x14ac:dyDescent="0.2">
@@ -6827,13 +6800,13 @@
         <v>135</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="240" x14ac:dyDescent="0.2">
@@ -6853,13 +6826,13 @@
         <v>135</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="144" x14ac:dyDescent="0.2">
@@ -6879,13 +6852,13 @@
         <v>135</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -6905,13 +6878,13 @@
         <v>135</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -6934,10 +6907,10 @@
         <v>256</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="335" x14ac:dyDescent="0.2">
@@ -6956,14 +6929,14 @@
       <c r="E134" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F134" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="H134" s="2" t="s">
-        <v>434</v>
+      <c r="F134" s="2">
+        <v>45.5</v>
+      </c>
+      <c r="G134" s="2">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="H134" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="272" x14ac:dyDescent="0.2">
@@ -6983,13 +6956,13 @@
         <v>135</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -7012,10 +6985,10 @@
         <v>259</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="192" x14ac:dyDescent="0.2">
@@ -7035,13 +7008,13 @@
         <v>135</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="395" x14ac:dyDescent="0.2">
@@ -7061,13 +7034,13 @@
         <v>135</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -7087,13 +7060,13 @@
         <v>135</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="224" x14ac:dyDescent="0.2">
@@ -7139,13 +7112,13 @@
         <v>135</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="304" x14ac:dyDescent="0.2">
@@ -7165,13 +7138,13 @@
         <v>135</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>